<commit_message>
Fixed date must be DD/MM/YYYY
</commit_message>
<xml_diff>
--- a/sample/excel/Simple_Template.xlsx
+++ b/sample/excel/Simple_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khair\Documents\GitHub\repositories\rendr\sample\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Lee\Documents\GitHub\rendr\sample\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF896E1-41C0-494C-9966-58722B428472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3101E80-6AB1-4D87-A8E1-DDC241C60B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="1095" windowWidth="19410" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holdings" sheetId="1" r:id="rId1"/>
@@ -146,43 +146,43 @@
     <t>marketValue</t>
   </si>
   <si>
-    <t>!! positionDate</t>
-  </si>
-  <si>
-    <t>!! instrumentType</t>
-  </si>
-  <si>
-    <t>!! ISIN</t>
-  </si>
-  <si>
-    <t>!! ticker</t>
-  </si>
-  <si>
-    <t>!! contractCode</t>
-  </si>
-  <si>
-    <t>!! coupon</t>
-  </si>
-  <si>
-    <t>!! maturityDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">!! currency </t>
-  </si>
-  <si>
-    <t>!! currentFace</t>
-  </si>
-  <si>
-    <t>!! originalFace</t>
-  </si>
-  <si>
-    <t>!! marketValue</t>
-  </si>
-  <si>
-    <t>!! price</t>
-  </si>
-  <si>
-    <t>!! portfolio</t>
+    <t>!!v positionDate</t>
+  </si>
+  <si>
+    <t>!!v portfolio</t>
+  </si>
+  <si>
+    <t>!!v instrumentType</t>
+  </si>
+  <si>
+    <t>!!v ISIN</t>
+  </si>
+  <si>
+    <t>!!v ticker</t>
+  </si>
+  <si>
+    <t>!!v contractCode</t>
+  </si>
+  <si>
+    <t>!!v coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!!v currency </t>
+  </si>
+  <si>
+    <t>!!v currentFace</t>
+  </si>
+  <si>
+    <t>!!v originalFace</t>
+  </si>
+  <si>
+    <t>!!v price</t>
+  </si>
+  <si>
+    <t>!!v marketValue</t>
+  </si>
+  <si>
+    <t>!!v maturityDate ++</t>
   </si>
 </sst>
 </file>
@@ -609,6 +609,9 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="4" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -617,9 +620,6 @@
     </xf>
     <xf numFmtId="165" fontId="10" fillId="4" borderId="6" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="19" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -1090,25 +1090,25 @@
         <v>40</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>46</v>
       </c>
       <c r="I2" s="27" t="s">
         <v>47</v>
@@ -1120,10 +1120,10 @@
         <v>49</v>
       </c>
       <c r="L2" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="31" t="s">
         <v>51</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="32" customFormat="1" ht="12.75" customHeight="1">
@@ -3340,13 +3340,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="41" t="s">
@@ -3397,132 +3397,125 @@
       <c r="A7" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:E12"/>
@@ -3533,6 +3526,13 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>